<commit_message>
updata DBHAPI_Variabler Excel with new filter and group by for tables 704, 705, 706, 707, 123, 124
</commit_message>
<xml_diff>
--- a/inst/extdata/DBHAPI_Variabler.xlsx
+++ b/inst/extdata/DBHAPI_Variabler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prosjekter\rdbhapi\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB81B9E-5873-4743-9726-0979FCB71B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E22350E-EDA4-479D-8F48-7FB12BC6E7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B1BD8177-F654-43D1-BDE5-BD46B37F9230}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
   <si>
     <t>Tabell id</t>
   </si>
@@ -203,12 +203,6 @@
     <t>Fagskolens navn,Utdanningstilbudets navn,Årstall, Semesternavn</t>
   </si>
   <si>
-    <t>Institusjonskode,Avdkode,Årstall</t>
-  </si>
-  <si>
-    <t>Institusjonskode,Avdkode,Årstall, Semester,Kjønnkode</t>
-  </si>
-  <si>
     <t>Institusjonskode,Avdelingskode,Avdelingsnavn,Årstall</t>
   </si>
   <si>
@@ -278,10 +272,22 @@
     <t>Institusjonskode,Avdelingskode,Årstall,Semester,Kvalifikasjonskode</t>
   </si>
   <si>
-    <t>Institusjonskode,Avdelingskode,Årstall,Semester,Studentkategori,Studieprogramkode,Studieretningkode,Stedkode campus</t>
-  </si>
-  <si>
-    <t>Institusjonskode,Avdelingskode,Årstall,Stedkode campus</t>
+    <t>Institusjonskode,Avdkode, Studiumkode,Årstall</t>
+  </si>
+  <si>
+    <t>Institusjonskode,Avdkode, Studiumkode,Årstall, Semester,Kjønnkode</t>
+  </si>
+  <si>
+    <t>Institusjonskode,Avdelingskode, Studiumkode,Årstall</t>
+  </si>
+  <si>
+    <t>Institusjonskode,Avdelingskode,Studiumkode,Årstall,Semester,Studentkategori</t>
+  </si>
+  <si>
+    <t>Institusjonskode,Avdelingskode,Studiumkode,Årstall,Stedkode campus</t>
+  </si>
+  <si>
+    <t>Institusjonskode,Avdelingskode,Studiumkode,Årstall,Semester,Studentkategori,Studieprogramkode,Studieretningkode,Stedkode campus</t>
   </si>
 </sst>
 </file>
@@ -674,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE6BF3C-3E67-48B4-9CCD-027E177EAA24}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,10 +764,10 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -778,10 +784,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -798,10 +804,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -818,10 +824,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -838,10 +844,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -858,10 +864,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -878,10 +884,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -898,7 +904,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -915,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -932,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -949,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -966,7 +972,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -983,10 +989,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1003,10 +1009,10 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1023,10 +1029,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
         <v>67</v>
-      </c>
-      <c r="F18" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1043,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1114,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1148,10 +1154,10 @@
         <v>0</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1168,10 +1174,10 @@
         <v>0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1188,7 +1194,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1205,10 +1211,10 @@
         <v>0</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1225,10 +1231,10 @@
         <v>0</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1245,10 +1251,10 @@
         <v>0</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1299,10 +1305,10 @@
         <v>0</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1319,10 +1325,10 @@
         <v>0</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1339,10 +1345,10 @@
         <v>0</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1359,10 +1365,10 @@
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1379,10 +1385,10 @@
         <v>0</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1399,10 +1405,10 @@
         <v>0</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1436,10 +1442,10 @@
         <v>0</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1456,10 +1462,10 @@
         <v>0</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>